<commit_message>
creacion de plantillas craga masiva
</commit_message>
<xml_diff>
--- a/gestion-talento-web/src/main/resources/static/files/PlantillaCargaMasiva.xlsx
+++ b/gestion-talento-web/src/main/resources/static/files/PlantillaCargaMasiva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\Proyecto\gestion-talento-web\src\main\resources\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\Proyecto\Proyecto\gestion-talento-web\src\main\resources\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,47 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Tipo Documento</t>
+  </si>
+  <si>
+    <t>Primer nombre</t>
+  </si>
+  <si>
+    <t>Segundo Nombre</t>
+  </si>
+  <si>
+    <t>Primer Apellido</t>
+  </si>
+  <si>
+    <t>Segundo Apellido</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Correo Electronico</t>
+  </si>
+  <si>
+    <t>Numero de documento</t>
+  </si>
+  <si>
+    <t>Codigo usuario</t>
+  </si>
+  <si>
+    <t>Jefe</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Tipo Usuario</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,8 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +380,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>